<commit_message>
[Mod] Reaction Data Cell 수정
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Data/Excels/ReactionData.xlsx
+++ b/Assets/Scripts/Data/Excels/ReactionData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\game\icecream\Assets\Scripts\Data\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceTree0115\Project_IceCream\Assets\Scripts\Data\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54592700-1B1B-4727-9B6C-357E47685358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4413BA83-8822-4CA4-B154-DDC71C905B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="1995" windowWidth="20760" windowHeight="11385" xr2:uid="{5B37F34A-57A3-4703-A322-362AC2538767}"/>
+    <workbookView xWindow="-16755" yWindow="7710" windowWidth="28800" windowHeight="15435" xr2:uid="{5B37F34A-57A3-4703-A322-362AC2538767}"/>
   </bookViews>
   <sheets>
     <sheet name="ReactionDatas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>ActionType</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,7 +50,79 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>와 맛있어요!</t>
+    <t>아..! 살 것 같다..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감사합니다! 정말 맛있어 보이네요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>둘이 먹다 하나 쪄 죽어도 모를 맛!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와! 이게 아이스크림이구나!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">최고에요! </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감사합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 다른 것 같은데.. 그래도 잘 먹을게요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 먹겠습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음.. 이런 맛이구나.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛있네요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이게.. 맞나요..?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에잉 이게 아닌데..쯧..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐야.. 장사할 생각 없어요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 아이스크림이 아니야!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이럴거면 주문 왜 받은거죠?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perfecct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,20 +487,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8EE5E7-4618-43EB-9D59-741AF98BFBB8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="36.375" customWidth="1"/>
     <col min="3" max="3" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,16 +510,218 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
         <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1.5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>